<commit_message>
Renommage du fichier Get-ExcelCellInfo en Create-AutoEvals et optimisation de code
</commit_message>
<xml_diff>
--- a/DataFiles/01-configs-auto-eval.xlsx
+++ b/DataFiles/01-configs-auto-eval.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42025B80-8C32-4C8F-BC39-34B2E36B18EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438C89C5-1CC5-454B-98AE-E4402DE906E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
   </bookViews>
   <sheets>
-    <sheet name="inputs" sheetId="3" r:id="rId1"/>
+    <sheet name="configs" sheetId="3" r:id="rId1"/>
     <sheet name="students" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -81,22 +81,22 @@
     <t>Bolli</t>
   </si>
   <si>
+    <t>Gilbert Gruaz</t>
+  </si>
+  <si>
+    <t>CIN4b</t>
+  </si>
+  <si>
+    <t>Champs</t>
+  </si>
+  <si>
+    <t>Valeurs</t>
+  </si>
+  <si>
+    <t>Date debut</t>
+  </si>
+  <si>
     <t>P_Appro</t>
-  </si>
-  <si>
-    <t>Gilbert Gruaz</t>
-  </si>
-  <si>
-    <t>CIN4b</t>
-  </si>
-  <si>
-    <t>Champs</t>
-  </si>
-  <si>
-    <t>Valeurs</t>
-  </si>
-  <si>
-    <t>Date debut</t>
   </si>
 </sst>
 </file>
@@ -452,17 +452,17 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,12 +478,12 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>44949</v>
@@ -518,7 +518,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add array in config file
</commit_message>
<xml_diff>
--- a/DataFiles/01-configs-auto-eval.xlsx
+++ b/DataFiles/01-configs-auto-eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438C89C5-1CC5-454B-98AE-E4402DE906E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49AC823-B025-4F59-BE2C-1BE3C62BBC49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
   </bookViews>
   <sheets>
     <sheet name="configs" sheetId="3" r:id="rId1"/>
@@ -132,14 +132,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -150,6 +159,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40A9120E-277B-491D-A705-693FEBE7DBB8}" name="Tableau1" displayName="Tableau1" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{571A42B8-CD2B-491E-A1C4-AEF2EEF4E918}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D4AFE5C8-9FD4-4B65-B290-B901D81F9C06}" name="Champs"/>
+    <tableColumn id="2" xr3:uid="{83C424F4-AEB1-45D0-8148-912FD27F0C12}" name="Valeurs" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4087EB84-0BC7-4AF6-BAFC-FAFA3D45A1A4}" name="Tableau2" displayName="Tableau2" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{BC065993-1B94-4FCA-95A9-FCB563A546A6}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A50D2CFF-5B68-476A-9BD6-6534906C740A}" name="Nom"/>
+    <tableColumn id="2" xr3:uid="{99EC5369-92B6-4282-9F75-711C8F12AFA5}" name="Prenom"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,11 +482,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A680B354-E400-4890-989B-5DBD9C1F0966}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -469,7 +504,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -477,7 +512,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -485,7 +520,7 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>44949</v>
       </c>
     </row>
@@ -493,7 +528,7 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>45009</v>
       </c>
     </row>
@@ -501,7 +536,7 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>300</v>
       </c>
     </row>
@@ -509,7 +544,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>10</v>
       </c>
     </row>
@@ -517,7 +552,7 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -525,12 +560,15 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -538,11 +576,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BBCFFD-9086-4D11-B5E2-D769F6D9E5FA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -578,5 +619,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mise en commun des AutoEvals dans un seul fichier
</commit_message>
<xml_diff>
--- a/DataFiles/01-configs-auto-eval.xlsx
+++ b/DataFiles/01-configs-auto-eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49AC823-B025-4F59-BE2C-1BE3C62BBC49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587EF1DB-5701-4D5E-BA2B-28647C1ACE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
   </bookViews>
   <sheets>
     <sheet name="configs" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Nom du projet</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>P_Appro</t>
+  </si>
+  <si>
+    <t>Visa Enseignant</t>
+  </si>
+  <si>
+    <t>GGZ</t>
   </si>
 </sst>
 </file>
@@ -162,8 +168,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40A9120E-277B-491D-A705-693FEBE7DBB8}" name="Tableau1" displayName="Tableau1" ref="A1:B9" totalsRowShown="0">
-  <autoFilter ref="A1:B9" xr:uid="{571A42B8-CD2B-491E-A1C4-AEF2EEF4E918}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{40A9120E-277B-491D-A705-693FEBE7DBB8}" name="Tableau1" displayName="Tableau1" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{571A42B8-CD2B-491E-A1C4-AEF2EEF4E918}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D4AFE5C8-9FD4-4B65-B290-B901D81F9C06}" name="Champs"/>
     <tableColumn id="2" xr3:uid="{83C424F4-AEB1-45D0-8148-912FD27F0C12}" name="Valeurs" dataDxfId="0"/>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A680B354-E400-4890-989B-5DBD9C1F0966}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,49 +524,57 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44949</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>45009</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>300</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45009</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>10</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
     </row>
@@ -576,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BBCFFD-9086-4D11-B5E2-D769F6D9E5FA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout de la synthèse automatique des notes
</commit_message>
<xml_diff>
--- a/DataFiles/01-configs-auto-eval.xlsx
+++ b/DataFiles/01-configs-auto-eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587EF1DB-5701-4D5E-BA2B-28647C1ACE72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B799A44B-6C82-4B0B-BA6D-4EA4713EB7F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
   </bookViews>
   <sheets>
     <sheet name="configs" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Nom du projet</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>GGZ</t>
+  </si>
+  <si>
+    <t>Younes</t>
+  </si>
+  <si>
+    <t>Sayeh</t>
+  </si>
+  <si>
+    <t>Philipona</t>
+  </si>
+  <si>
+    <t>Sylvain</t>
   </si>
 </sst>
 </file>
@@ -179,8 +191,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4087EB84-0BC7-4AF6-BAFC-FAFA3D45A1A4}" name="Tableau2" displayName="Tableau2" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{BC065993-1B94-4FCA-95A9-FCB563A546A6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4087EB84-0BC7-4AF6-BAFC-FAFA3D45A1A4}" name="Tableau2" displayName="Tableau2" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{BC065993-1B94-4FCA-95A9-FCB563A546A6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A50D2CFF-5B68-476A-9BD6-6534906C740A}" name="Nom"/>
     <tableColumn id="2" xr3:uid="{99EC5369-92B6-4282-9F75-711C8F12AFA5}" name="Prenom"/>
@@ -488,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A680B354-E400-4890-989B-5DBD9C1F0966}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,10 +600,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BBCFFD-9086-4D11-B5E2-D769F6D9E5FA}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,6 +643,22 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>